<commit_message>
push small exp seq edits
</commit_message>
<xml_diff>
--- a/examples/sequences/q2d_rf_pulse_sequence.xlsx
+++ b/examples/sequences/q2d_rf_pulse_sequence.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\GitHub\chip-lab\ChiPyLab\examples\sequences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coldatoms\Documents\cjdGitHub\ChiPyLab\examples\sequences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3BF58C-9ECE-4ADF-BE79-7915F7324CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{D818C0C5-7768-4858-97A0-2DC1B457CA77}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,8 +94,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,24 +459,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012E0891-FB82-47F4-804A-8621778D1A0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="C2">
         <v>1</v>
       </c>
@@ -511,13 +510,13 @@
         <v>14</v>
       </c>
       <c r="F2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -534,7 +533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -551,7 +550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -565,12 +564,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="C6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -587,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="C8">
         <v>1</v>
       </c>

</xml_diff>